<commit_message>
Zoe submit new scripts
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.40.20.10_PermissionForNewActionOfEachGroup.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.40.20.10_PermissionForNewActionOfEachGroup.xlsx
@@ -4808,8 +4808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F139" sqref="F139"/>
+    <sheetView tabSelected="1" topLeftCell="D43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6808,7 +6808,7 @@
         <v>833</v>
       </c>
       <c r="J73" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K73" s="20"/>
       <c r="L73" s="20"/>

</xml_diff>